<commit_message>
adding content on due dates, grace period
</commit_message>
<xml_diff>
--- a/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
+++ b/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85df9cffced7e2ed/Documents/github/tracigardner.github.io/TechComm/semester/2025-08-Fall/check-in-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D3E35D-C95A-4853-B462-EC3D1FC0141A}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="2" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
+    <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="1" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 Check-In Survey Survey S" sheetId="1" r:id="rId1"/>
@@ -1166,7 +1166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1352,6 +1352,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1513,7 +1519,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1531,6 +1537,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7379,8 +7395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372C75A9-AE31-4732-89CF-5AB25AC857A4}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7506,19 +7522,19 @@
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:2" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="8" t="s">
         <v>312</v>
       </c>
     </row>
@@ -8023,8 +8039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA16309E-9085-4226-83B5-5B0683BB2692}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8102,19 +8118,19 @@
         <v>263</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="8" t="s">
         <v>273</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on topic announcement
</commit_message>
<xml_diff>
--- a/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
+++ b/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85df9cffced7e2ed/Documents/github/tracigardner.github.io/TechComm/semester/2025-08-Fall/check-in-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D3E35D-C95A-4853-B462-EC3D1FC0141A}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADB55F89-23AA-4E93-80FD-60C959D83D17}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="1" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
   </bookViews>
@@ -7395,8 +7395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372C75A9-AE31-4732-89CF-5AB25AC857A4}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7410,11 +7410,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>298</v>
       </c>
     </row>
@@ -7434,19 +7434,19 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="8" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7506,11 +7506,11 @@
         <v>306</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="8" t="s">
         <v>325</v>
       </c>
     </row>
@@ -7570,11 +7570,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="8" t="s">
         <v>289</v>
       </c>
     </row>
@@ -7602,11 +7602,11 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:2" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="8" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7650,35 +7650,35 @@
         <v>293</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:2" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="8" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:2" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="8" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:2" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="8" t="s">
         <v>307</v>
       </c>
     </row>
@@ -7706,19 +7706,19 @@
         <v>274</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="8" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="8" t="s">
         <v>322</v>
       </c>
     </row>
@@ -7778,19 +7778,19 @@
         <v>291</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:2" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="8" t="s">
         <v>303</v>
       </c>
     </row>
@@ -7850,11 +7850,11 @@
         <v>300</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:2" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="8" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7874,11 +7874,11 @@
         <v>329</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:2" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="8" t="s">
         <v>275</v>
       </c>
     </row>
@@ -7906,19 +7906,19 @@
         <v>328</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="8" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="8" t="s">
         <v>281</v>
       </c>
     </row>
@@ -8040,7 +8040,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8070,19 +8070,19 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding dates and weights to project overview; additional content to faq; adding announcement modified from JM's
</commit_message>
<xml_diff>
--- a/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
+++ b/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85df9cffced7e2ed/Documents/github/tracigardner.github.io/TechComm/semester/2025-08-Fall/check-in-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADB55F89-23AA-4E93-80FD-60C959D83D17}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BFF3C5E-BA92-4978-93B0-EDF09D08E631}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="1" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
+    <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="2" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 Check-In Survey Survey S" sheetId="1" r:id="rId1"/>
@@ -1607,6 +1607,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7395,8 +7399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372C75A9-AE31-4732-89CF-5AB25AC857A4}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7450,35 +7454,35 @@
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="8" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="8" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="8" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:2" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>313</v>
       </c>
     </row>
@@ -7738,19 +7742,19 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="8" t="s">
         <v>276</v>
       </c>
     </row>
@@ -8039,8 +8043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA16309E-9085-4226-83B5-5B0683BB2692}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8086,19 +8090,19 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="8" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:2" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="8" t="s">
         <v>267</v>
       </c>
     </row>
@@ -8110,11 +8114,11 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:2" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="8" t="s">
         <v>263</v>
       </c>
     </row>
@@ -8158,11 +8162,11 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="8" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more content; adding textbook to course homepage useful links
</commit_message>
<xml_diff>
--- a/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
+++ b/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85df9cffced7e2ed/Documents/github/tracigardner.github.io/TechComm/semester/2025-08-Fall/check-in-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BFF3C5E-BA92-4978-93B0-EDF09D08E631}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{96F4182B-DEA1-4504-9054-BDC6FC8FD003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AC61B5-9990-4E99-A7EE-79D31B25C8B4}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="2" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
+    <workbookView xWindow="345" yWindow="810" windowWidth="26280" windowHeight="13950" activeTab="1" xr2:uid="{AAD23576-8FB9-4CBF-ABFA-C0E08058CEAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 Check-In Survey Survey S" sheetId="1" r:id="rId1"/>
@@ -1166,7 +1166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1358,6 +1358,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1519,7 +1531,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1549,6 +1561,20 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7399,8 +7425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372C75A9-AE31-4732-89CF-5AB25AC857A4}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7486,27 +7512,27 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:2" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="12" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="12" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:2" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="12" t="s">
         <v>306</v>
       </c>
     </row>
@@ -7518,11 +7544,11 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:2" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="12" t="s">
         <v>314</v>
       </c>
     </row>
@@ -7542,27 +7568,27 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:2" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="15" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:2" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="12" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="12" t="s">
         <v>287</v>
       </c>
     </row>
@@ -8043,7 +8069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA16309E-9085-4226-83B5-5B0683BB2692}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working on design for anno
</commit_message>
<xml_diff>
--- a/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
+++ b/TechComm/semester/2025-08-Fall/check-in-analysis/Week 1 Check-In Survey Survey Student Analysis Report.xlsx
@@ -7438,8 +7438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372C75A9-AE31-4732-89CF-5AB25AC857A4}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8083,8 +8083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA16309E-9085-4226-83B5-5B0683BB2692}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>